<commit_message>
stats collected for scores graphing
</commit_message>
<xml_diff>
--- a/Neighbourhood Weightings.xlsx
+++ b/Neighbourhood Weightings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jusxp\Desktop\UBC\UT Grad School\Systems Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DFA16F2-5C7E-4F91-8C1B-D4AB85A414AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE3C889-83E3-42D2-ABDD-B732FF4E0F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DBA2EB4A-0C92-4544-87CA-C532A95C4B64}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DBA2EB4A-0C92-4544-87CA-C532A95C4B64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -264,11 +264,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -281,46 +317,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -400,16 +397,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>44835</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>38035</xdr:rowOff>
+      <xdr:colOff>149610</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>171385</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -432,7 +429,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7077075" y="1647825"/>
+          <a:off x="7181850" y="1590675"/>
           <a:ext cx="3292860" cy="5057710"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -800,331 +797,331 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="13" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="13" t="s">
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="13" t="s">
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="13" t="s">
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="15"/>
-      <c r="U3" s="16"/>
-      <c r="V3" s="13" t="s">
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="15"/>
+      <c r="W3" s="12"/>
+      <c r="X3" s="12"/>
+      <c r="Y3" s="13"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="8" t="s">
+      <c r="A4" s="10"/>
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="8" t="s">
+      <c r="E4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" s="17"/>
-      <c r="L4" s="8" t="s">
+      <c r="J4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="10"/>
+      <c r="L4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="M4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="N4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="8" t="s">
+      <c r="O4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="R4" s="9" t="s">
+      <c r="R4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="S4" s="9" t="s">
+      <c r="S4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="T4" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="U4" s="17"/>
-      <c r="V4" s="8" t="s">
+      <c r="T4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="U4" s="10"/>
+      <c r="V4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="W4" s="9" t="s">
+      <c r="W4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="X4" s="9" t="s">
+      <c r="X4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="Y4" s="10" t="s">
+      <c r="Y4" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="2">
         <v>8</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="1">
         <v>2</v>
       </c>
-      <c r="D5" s="6">
-        <v>7</v>
-      </c>
-      <c r="E5" s="7">
+      <c r="D5" s="1">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3">
         <v>10</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="2">
         <v>9</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="1">
         <v>2</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="1">
         <v>9</v>
       </c>
-      <c r="J5" s="7">
-        <v>7</v>
-      </c>
-      <c r="K5" s="11" t="s">
+      <c r="J5" s="3">
+        <v>7</v>
+      </c>
+      <c r="K5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="2">
         <v>2</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="1">
         <v>10</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N5" s="1">
         <v>9</v>
       </c>
-      <c r="O5" s="7">
+      <c r="O5" s="3">
         <v>10</v>
       </c>
-      <c r="P5" s="11" t="s">
+      <c r="P5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="Q5" s="2" t="s">
+      <c r="Q5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="11" t="s">
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="V5" s="5">
+      <c r="V5" s="2">
         <v>6</v>
       </c>
-      <c r="W5" s="6">
+      <c r="W5" s="1">
         <v>6</v>
       </c>
-      <c r="X5" s="6">
+      <c r="X5" s="1">
         <v>6</v>
       </c>
-      <c r="Y5" s="7">
+      <c r="Y5" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="2">
         <v>10</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="1">
         <v>8</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="1">
         <v>9</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="3">
         <v>8</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="2">
         <v>10</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="1">
         <v>8</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="1">
         <v>10</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="3">
         <v>6</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="2">
         <v>2</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="1">
         <v>10</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N6" s="1">
         <v>9</v>
       </c>
-      <c r="O6" s="7">
+      <c r="O6" s="3">
         <v>10</v>
       </c>
-      <c r="P6" s="11" t="s">
+      <c r="P6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="19"/>
-      <c r="S6" s="19"/>
-      <c r="T6" s="20"/>
-      <c r="U6" s="11" t="s">
+      <c r="Q6" s="17"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="V6" s="5">
-        <v>7</v>
-      </c>
-      <c r="W6" s="6">
-        <v>7</v>
-      </c>
-      <c r="X6" s="6">
-        <v>7</v>
-      </c>
-      <c r="Y6" s="7">
+      <c r="V6" s="2">
+        <v>7</v>
+      </c>
+      <c r="W6" s="1">
+        <v>7</v>
+      </c>
+      <c r="X6" s="1">
+        <v>7</v>
+      </c>
+      <c r="Y6" s="3">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="8">
-        <v>7</v>
-      </c>
-      <c r="C7" s="9">
+      <c r="B7" s="4">
+        <v>7</v>
+      </c>
+      <c r="C7" s="5">
         <v>8</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="5">
         <v>4</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="6">
         <v>1</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="8">
-        <v>7</v>
-      </c>
-      <c r="H7" s="9">
+      <c r="G7" s="4">
+        <v>7</v>
+      </c>
+      <c r="H7" s="5">
         <v>4</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="5">
         <v>4</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="6">
         <v>1</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7" s="4">
         <v>2</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M7" s="5">
         <v>10</v>
       </c>
-      <c r="N7" s="9">
+      <c r="N7" s="5">
         <v>9</v>
       </c>
-      <c r="O7" s="10">
+      <c r="O7" s="6">
         <v>10</v>
       </c>
-      <c r="P7" s="12" t="s">
+      <c r="P7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="22"/>
-      <c r="S7" s="22"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="12" t="s">
+      <c r="Q7" s="20"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="22"/>
+      <c r="U7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="V7" s="8">
+      <c r="V7" s="4">
         <v>9</v>
       </c>
-      <c r="W7" s="9">
+      <c r="W7" s="5">
         <v>9</v>
       </c>
-      <c r="X7" s="9">
+      <c r="X7" s="5">
         <v>9</v>
       </c>
-      <c r="Y7" s="10">
+      <c r="Y7" s="6">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="Q5:T7"/>
+    <mergeCell ref="V3:Y3"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="Q3:T3"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="P3:P4"/>
     <mergeCell ref="U3:U4"/>
-    <mergeCell ref="V3:Y3"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="L3:O3"/>
-    <mergeCell ref="Q3:T3"/>
-    <mergeCell ref="Q5:T7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>